<commit_message>
Tests for IF = <> TRUE FALSE
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t xml:space="preserve">rectangular range</t>
   </si>
@@ -43,6 +43,42 @@
   </si>
   <si>
     <t xml:space="preserve">formula references another sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'&lt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'&gt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if / true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if / false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if / true with no else</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if / false with no else</t>
+  </si>
+  <si>
+    <t xml:space="preserve">always true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">always false</t>
   </si>
   <si>
     <t xml:space="preserve">total</t>
@@ -67,12 +103,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="167" formatCode="hh:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="168" formatCode="hh:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="169" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -97,7 +134,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,8 +147,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEE7E5"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -172,6 +215,13 @@
       <left/>
       <right style="hair"/>
       <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
@@ -222,11 +272,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -267,12 +321,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -288,6 +358,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -336,7 +410,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFDEE7E5"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -368,281 +442,281 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>-80.1</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <f aca="false">A2*2</f>
         <v>-160.2</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <f aca="false">B2*2</f>
         <v>-320.4</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <f aca="false">C2*2</f>
         <v>-640.8</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <f aca="false">D2*2</f>
         <v>-1281.6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
+      <c r="A3" s="5" t="n">
         <f aca="false">A2+20.1</f>
         <v>-60</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="6" t="n">
         <f aca="false">A3*2</f>
         <v>-120</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="6" t="n">
         <f aca="false">B3*2</f>
         <v>-240</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="6" t="n">
         <f aca="false">C3*2</f>
         <v>-480</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="7" t="n">
         <f aca="false">D3*2</f>
         <v>-960</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
+      <c r="A4" s="5" t="n">
         <f aca="false">A3+20.1</f>
         <v>-39.9</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="6" t="n">
         <f aca="false">A4*2</f>
         <v>-79.8</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="6" t="n">
         <f aca="false">B4*2</f>
         <v>-159.6</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="6" t="n">
         <f aca="false">C4*2</f>
         <v>-319.2</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="7" t="n">
         <f aca="false">D4*2</f>
         <v>-638.4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="5" t="n">
         <f aca="false">A4+20.1</f>
         <v>-19.8</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="6" t="n">
         <f aca="false">A5*2</f>
         <v>-39.6</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <f aca="false">B5*2</f>
         <v>-79.2</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="6" t="n">
         <f aca="false">C5*2</f>
         <v>-158.4</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="7" t="n">
         <f aca="false">D5*2</f>
         <v>-316.8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
+      <c r="A6" s="5" t="n">
         <f aca="false">A5+20.1</f>
         <v>0.300000000000011</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="6" t="n">
         <f aca="false">A6*2</f>
         <v>0.600000000000023</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="6" t="n">
         <f aca="false">B6*2</f>
         <v>1.20000000000005</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="6" t="n">
         <f aca="false">C6*2</f>
         <v>2.40000000000009</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="7" t="n">
         <f aca="false">D6*2</f>
         <v>4.80000000000018</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="5" t="n">
         <f aca="false">A6+20.1</f>
         <v>20.4</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="6" t="n">
         <f aca="false">A7*2</f>
         <v>40.8</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="6" t="n">
         <f aca="false">B7*2</f>
         <v>81.6000000000001</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="6" t="n">
         <f aca="false">C7*2</f>
         <v>163.2</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="7" t="n">
         <f aca="false">D7*2</f>
         <v>326.4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
+      <c r="A8" s="5" t="n">
         <f aca="false">A7+20.1</f>
         <v>40.5</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="6" t="n">
         <f aca="false">A8*2</f>
         <v>81</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <f aca="false">B8*2</f>
         <v>162</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="6" t="n">
         <f aca="false">C8*2</f>
         <v>324</v>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E8" s="7" t="n">
         <f aca="false">D8*2</f>
         <v>648</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
+      <c r="A9" s="5" t="n">
         <f aca="false">A8+20.1</f>
         <v>60.6</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="6" t="n">
         <f aca="false">A9*2</f>
         <v>121.2</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="6" t="n">
         <f aca="false">B9*2</f>
         <v>242.4</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="6" t="n">
         <f aca="false">C9*2</f>
         <v>484.8</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="7" t="n">
         <f aca="false">D9*2</f>
         <v>969.6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
+      <c r="A10" s="5" t="n">
         <f aca="false">A9+20.1</f>
         <v>80.7</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="6" t="n">
         <f aca="false">A10*2</f>
         <v>161.4</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="6" t="n">
         <f aca="false">B10*2</f>
         <v>322.8</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="6" t="n">
         <f aca="false">C10*2</f>
         <v>645.6</v>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="7" t="n">
         <f aca="false">D10*2</f>
         <v>1291.2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
+      <c r="A11" s="8" t="n">
         <f aca="false">A10+20.1</f>
         <v>100.8</v>
       </c>
-      <c r="B11" s="8" t="n">
+      <c r="B11" s="9" t="n">
         <f aca="false">A11*2</f>
         <v>201.6</v>
       </c>
-      <c r="C11" s="8" t="n">
+      <c r="C11" s="9" t="n">
         <f aca="false">B11*2</f>
         <v>403.2</v>
       </c>
-      <c r="D11" s="8" t="n">
+      <c r="D11" s="9" t="n">
         <f aca="false">C11*2</f>
         <v>806.4</v>
       </c>
-      <c r="E11" s="9" t="n">
+      <c r="E11" s="10" t="n">
         <f aca="false">D11*2</f>
         <v>1612.8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <f aca="false">MIN(A2:E11)</f>
         <v>-1281.6</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <f aca="false">MAX(A2:E11)</f>
         <v>1612.8</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <f aca="false">AVERAGE(A2:E11)</f>
         <v>64.1700000000001</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <f aca="false">SUM(A2:E11)</f>
         <v>3208.5</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="11" t="n">
         <v>12</v>
       </c>
@@ -654,51 +728,260 @@
       <c r="F18" s="11" t="n">
         <v>56</v>
       </c>
-      <c r="G18" s="12"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <f aca="false">MIN(A18:G18)</f>
         <v>12</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <f aca="false">MAX(A18:G18)</f>
         <v>56</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <f aca="false">AVERAGE(A18:G18)</f>
         <v>34</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <f aca="false">SUM(A18:G18)</f>
         <v>102</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <f aca="false">2*Sheet2!A9</f>
         <v>356</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="15" t="n">
+        <f aca="false">$A$19=12</f>
+        <v>1</v>
+      </c>
+      <c r="B27" s="15" t="n">
+        <f aca="false">$A$19&lt;&gt;13</f>
+        <v>1</v>
+      </c>
+      <c r="C27" s="15" t="n">
+        <f aca="false">$A$19&lt;13</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="15" t="n">
+        <f aca="false">$A$19&lt;=12</f>
+        <v>1</v>
+      </c>
+      <c r="E27" s="15" t="n">
+        <f aca="false">$A$19&gt;11</f>
+        <v>1</v>
+      </c>
+      <c r="F27" s="15" t="n">
+        <f aca="false">$A$19&gt;=12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="15" t="n">
+        <f aca="false">$A$19=13</f>
+        <v>0</v>
+      </c>
+      <c r="B28" s="15" t="n">
+        <f aca="false">$A$19&lt;&gt;12</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="15" t="n">
+        <f aca="false">$A$19&lt;12</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="15" t="n">
+        <f aca="false">$A$19&lt;=11</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="15" t="n">
+        <f aca="false">$A$19&gt;12</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="15" t="n">
+        <f aca="false">$A$19&gt;=13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="16" t="str">
+        <f aca="false">IF(A27,"yup","nope")</f>
+        <v>yup</v>
+      </c>
+      <c r="B29" s="16" t="str">
+        <f aca="false">IF(B27,"yup","nope")</f>
+        <v>yup</v>
+      </c>
+      <c r="C29" s="16" t="str">
+        <f aca="false">IF(C27,"yup","nope")</f>
+        <v>yup</v>
+      </c>
+      <c r="D29" s="16" t="str">
+        <f aca="false">IF(D27,"yup","nope")</f>
+        <v>yup</v>
+      </c>
+      <c r="E29" s="16" t="str">
+        <f aca="false">IF(E27,"yup","nope")</f>
+        <v>yup</v>
+      </c>
+      <c r="F29" s="16" t="str">
+        <f aca="false">IF(F27,"yup","nope")</f>
+        <v>yup</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="16" t="str">
+        <f aca="false">IF(A28,"nope","yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="B30" s="16" t="str">
+        <f aca="false">IF(B28,"nope","yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="C30" s="16" t="str">
+        <f aca="false">IF(C28,"nope","yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="D30" s="16" t="str">
+        <f aca="false">IF(D28,"nope","yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="E30" s="16" t="str">
+        <f aca="false">IF(E28,"nope","yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="F30" s="16" t="str">
+        <f aca="false">IF(F28,"nope","yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="16" t="str">
+        <f aca="false">IF(A27,"yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="B31" s="16" t="str">
+        <f aca="false">IF(B27,"yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="C31" s="16" t="str">
+        <f aca="false">IF(C27,"yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="D31" s="16" t="str">
+        <f aca="false">IF(D27,"yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="E31" s="16" t="str">
+        <f aca="false">IF(E27,"yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="F31" s="16" t="str">
+        <f aca="false">IF(F27,"yup")</f>
+        <v>yup</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="17" t="n">
+        <f aca="false">IF(A28,"nope")</f>
+        <v>0</v>
+      </c>
+      <c r="B32" s="17" t="n">
+        <f aca="false">IF(B28,"nope")</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="17" t="n">
+        <f aca="false">IF(C28,"nope")</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="17" t="n">
+        <f aca="false">IF(D28,"nope")</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="17" t="n">
+        <f aca="false">IF(E28,"nope")</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="17" t="n">
+        <f aca="false">IF(F28,"nope")</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="18"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="19" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -723,98 +1006,98 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="n">
         <f aca="false">'Foo Bar'!A1</f>
         <v>10</v>
       </c>
-      <c r="B1" s="0" t="str">
+      <c r="B1" s="1" t="str">
         <f aca="false">REPT("|",A1)</f>
         <v>||||||||||</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <f aca="false">A1+'Foo Bar'!$A$2</f>
         <v>13.5</v>
       </c>
-      <c r="B2" s="0" t="str">
+      <c r="B2" s="1" t="str">
         <f aca="false">REPT("|",A2)</f>
         <v>|||||||||||||</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <f aca="false">A2+'Foo Bar'!$A$2</f>
         <v>17</v>
       </c>
-      <c r="B3" s="0" t="str">
+      <c r="B3" s="1" t="str">
         <f aca="false">REPT("|",A3)</f>
         <v>|||||||||||||||||</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <f aca="false">A3+'Foo Bar'!$A$2</f>
         <v>20.5</v>
       </c>
-      <c r="B4" s="0" t="str">
+      <c r="B4" s="1" t="str">
         <f aca="false">REPT("|",A4)</f>
         <v>||||||||||||||||||||</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <f aca="false">A4+'Foo Bar'!$A$2</f>
         <v>24</v>
       </c>
-      <c r="B5" s="0" t="str">
+      <c r="B5" s="1" t="str">
         <f aca="false">REPT("|",A5)</f>
         <v>||||||||||||||||||||||||</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <f aca="false">A5+'Foo Bar'!$A$2</f>
         <v>27.5</v>
       </c>
-      <c r="B6" s="0" t="str">
+      <c r="B6" s="1" t="str">
         <f aca="false">REPT("|",A6)</f>
         <v>|||||||||||||||||||||||||||</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <f aca="false">A6+'Foo Bar'!$A$2</f>
         <v>31</v>
       </c>
-      <c r="B7" s="0" t="str">
+      <c r="B7" s="1" t="str">
         <f aca="false">REPT("|",A7)</f>
         <v>|||||||||||||||||||||||||||||||</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <f aca="false">A7+'Foo Bar'!$A$2</f>
         <v>34.5</v>
       </c>
-      <c r="B8" s="0" t="str">
+      <c r="B8" s="1" t="str">
         <f aca="false">REPT("|",A8)</f>
         <v>||||||||||||||||||||||||||||||||||</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <f aca="false">SUM(A1:A8)</f>
         <v>178</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>7</v>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -839,62 +1122,62 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>8</v>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>3.5</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>9</v>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="n">
+      <c r="A4" s="20" t="n">
         <v>44138</v>
       </c>
-      <c r="B4" s="14" t="n">
+      <c r="B4" s="19" t="n">
         <f aca="false">A4</f>
         <v>44138</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>10</v>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="n">
+      <c r="A5" s="21" t="n">
         <v>0.538352575862974</v>
       </c>
-      <c r="B5" s="14" t="n">
+      <c r="B5" s="19" t="n">
         <f aca="false">A5</f>
         <v>0.538352575862974</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>11</v>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="n">
+      <c r="A6" s="22" t="n">
         <v>44138.5383449074</v>
       </c>
-      <c r="B6" s="14" t="n">
+      <c r="B6" s="19" t="n">
         <f aca="false">A6</f>
         <v>44138.5383449074</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>12</v>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xlsx2py: Copy comments in .xlsx through to .py
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -19,6 +19,31 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">This cell A9 has
+A multi-line
+comment</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,7 +362,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -448,7 +473,7 @@
       <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -872,7 +897,7 @@
         <f aca="false">IF(F27,"yup","nope")</f>
         <v>yup</v>
       </c>
-      <c r="G29" s="0" t="s">
+      <c r="G29" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -901,7 +926,7 @@
         <f aca="false">IF(F28,"nope","yup")</f>
         <v>yup</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="G30" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -930,7 +955,7 @@
         <f aca="false">IF(F27,"yup")</f>
         <v>yup</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="G31" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -959,7 +984,7 @@
         <f aca="false">IF(F28,"nope")</f>
         <v>0</v>
       </c>
-      <c r="G32" s="0" t="s">
+      <c r="G32" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -980,7 +1005,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1003,10 +1028,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
   </cols>
@@ -1108,6 +1133,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1122,9 +1148,9 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.14"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
xlsx2py: ISFORMULA unit test
Also, add ISFORMULA function in Xlsx.py to be more consistent,
more clear and more flexible.
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t xml:space="preserve">rectangular range</t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t xml:space="preserve">always false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isformula – formula cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isformula – number cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isformula – text cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isformula – empty cell</t>
   </si>
   <si>
     <t xml:space="preserve">total</t>
@@ -297,7 +309,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -359,10 +371,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -467,13 +475,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -960,27 +968,27 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="17" t="n">
+      <c r="A32" s="16" t="n">
         <f aca="false">IF(A28,"nope")</f>
         <v>0</v>
       </c>
-      <c r="B32" s="17" t="n">
+      <c r="B32" s="16" t="n">
         <f aca="false">IF(B28,"nope")</f>
         <v>0</v>
       </c>
-      <c r="C32" s="17" t="n">
+      <c r="C32" s="16" t="n">
         <f aca="false">IF(C28,"nope")</f>
         <v>0</v>
       </c>
-      <c r="D32" s="17" t="n">
+      <c r="D32" s="16" t="n">
         <f aca="false">IF(D28,"nope")</f>
         <v>0</v>
       </c>
-      <c r="E32" s="17" t="n">
+      <c r="E32" s="16" t="n">
         <f aca="false">IF(E28,"nope")</f>
         <v>0</v>
       </c>
-      <c r="F32" s="17" t="n">
+      <c r="F32" s="16" t="n">
         <f aca="false">IF(F28,"nope")</f>
         <v>0</v>
       </c>
@@ -989,24 +997,60 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="18"/>
+      <c r="A33" s="17"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="19" t="n">
+      <c r="A34" s="18" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="19" t="n">
+      <c r="A35" s="18" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="18" t="n">
+        <f aca="false">_xlfn.ISFORMULA(A19)</f>
+        <v>1</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="18" t="n">
+        <f aca="false">_xlfn.ISFORMULA('Foo Bar'!A1)</f>
+        <v>0</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="18" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B37)</f>
+        <v>0</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="18" t="n">
+        <f aca="false">_xlfn.ISFORMULA(A36)</f>
+        <v>0</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1031,7 +1075,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
   </cols>
@@ -1122,7 +1166,7 @@
         <v>178</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1148,7 +1192,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.14"/>
@@ -1159,7 +1203,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,43 +1211,43 @@
         <v>3.5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="n">
+      <c r="A4" s="19" t="n">
         <v>44138</v>
       </c>
-      <c r="B4" s="19" t="n">
+      <c r="B4" s="18" t="n">
         <f aca="false">A4</f>
         <v>44138</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="n">
+      <c r="A5" s="20" t="n">
         <v>0.538352575862974</v>
       </c>
-      <c r="B5" s="19" t="n">
+      <c r="B5" s="18" t="n">
         <f aca="false">A5</f>
         <v>0.538352575862974</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="n">
+      <c r="A6" s="21" t="n">
         <v>44138.5383449074</v>
       </c>
-      <c r="B6" s="19" t="n">
+      <c r="B6" s="18" t="n">
         <f aca="false">A6</f>
         <v>44138.5383449074</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>